<commit_message>
update tree storage cost test
</commit_message>
<xml_diff>
--- a/docs/tree/tree_test.xlsx
+++ b/docs/tree/tree_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\File\Repo\cur\Ark-Searchable-Encryption\docs\tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\Repo\Ark-Encryption-Platform\docs\tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346EBB28-32F3-447F-992E-266009CFA606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358E9477-C52A-4E5F-8F29-3F519C481B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>维度\数据量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,6 +52,14 @@
   </si>
   <si>
     <t>索引建立（10次构建取平均）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对应存储开销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位 bytes</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -383,28 +391,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.88671875" customWidth="1"/>
+    <col min="1" max="1" width="50.875" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.875" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="16.25" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +434,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -448,7 +457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -469,7 +478,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -490,7 +499,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -498,141 +507,193 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F9" s="1">
+        <v>25000</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="1">
+        <v>200000</v>
+      </c>
+      <c r="C10" s="1">
+        <v>400000</v>
+      </c>
+      <c r="D10" s="1">
+        <v>600000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>800000</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1">
+        <v>200000</v>
+      </c>
+      <c r="C11" s="1">
+        <v>400000</v>
+      </c>
+      <c r="D11" s="1">
+        <v>600000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>800000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>200000</v>
+      </c>
+      <c r="C12" s="1">
+        <v>400000</v>
+      </c>
+      <c r="D12" s="1">
+        <v>600000</v>
+      </c>
+      <c r="E12" s="1">
+        <v>800000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B16" s="1">
         <v>5000</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C16" s="1">
         <v>10000</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D16" s="1">
         <v>15000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E16" s="1">
         <v>20000</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F16" s="1">
         <v>25000</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B17" s="1">
         <v>566</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C17" s="1">
         <v>579</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D17" s="1">
         <v>551</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E17" s="1">
         <v>558</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F17" s="1">
         <v>539</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B18" s="1">
         <v>544</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C18" s="1">
         <v>539</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D18" s="1">
         <v>561</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E18" s="1">
         <v>546</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F18" s="1">
         <v>551</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B19" s="1">
         <v>544</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C19" s="1">
         <v>546</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D19" s="1">
         <v>542</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E19" s="1">
         <v>549</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F19" s="1">
         <v>573</v>
       </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="G19" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>